<commit_message>
Added the parts for the results.
</commit_message>
<xml_diff>
--- a/Classification results.xlsx
+++ b/Classification results.xlsx
@@ -537,11 +537,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-834564768"/>
-        <c:axId val="-834570752"/>
+        <c:axId val="-702704992"/>
+        <c:axId val="-702720224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-834564768"/>
+        <c:axId val="-702704992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -584,7 +584,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-834570752"/>
+        <c:crossAx val="-702720224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -592,7 +592,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-834570752"/>
+        <c:axId val="-702720224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -644,7 +644,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-834564768"/>
+        <c:crossAx val="-702704992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -868,8 +868,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1061421632"/>
-        <c:axId val="-1061412384"/>
+        <c:axId val="-698612752"/>
+        <c:axId val="-698600240"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -976,7 +976,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$4</c15:sqref>
@@ -1003,7 +1003,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$2:$G$2</c15:sqref>
@@ -1035,7 +1035,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$4:$G$4</c15:sqref>
@@ -1074,7 +1074,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$5</c15:sqref>
@@ -1101,7 +1101,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$2:$G$2</c15:sqref>
@@ -1133,7 +1133,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$5:$G$5</c15:sqref>
@@ -1170,7 +1170,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1061421632"/>
+        <c:axId val="-698612752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1213,7 +1213,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1061412384"/>
+        <c:crossAx val="-698600240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1221,7 +1221,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1061412384"/>
+        <c:axId val="-698600240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1272,7 +1272,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1061421632"/>
+        <c:crossAx val="-698612752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2767,15 +2767,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G6"/>
+  <dimension ref="A2:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -2796,7 +2796,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -2818,8 +2818,12 @@
       <c r="G3" s="1">
         <v>0.90429999999999999</v>
       </c>
+      <c r="H3">
+        <f>AVERAGE(B3:G3)</f>
+        <v>0.90888333333333338</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -2841,8 +2845,12 @@
       <c r="G4" s="1">
         <v>0.73080000000000001</v>
       </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H6" si="0">AVERAGE(B4:G4)</f>
+        <v>0.66993333333333327</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -2864,8 +2872,12 @@
       <c r="G5" s="1">
         <v>0.82609999999999995</v>
       </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>0.7513333333333333</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -2874,24 +2886,28 @@
         <v>0.88695629317607416</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" ref="C6:G6" si="0">2 * (C4*C5) / (C4 + C5)</f>
+        <f t="shared" ref="C6:G6" si="1">2 * (C4*C5) / (C4 + C5)</f>
         <v>0.94736842105263164</v>
       </c>
       <c r="D6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.49999049599049605</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.2499414015843997</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.66669619073718833</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.77553327766715907</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="0"/>
-        <v>0.49999049599049605</v>
-      </c>
-      <c r="E6" s="1">
-        <f t="shared" si="0"/>
-        <v>0.2499414015843997</v>
-      </c>
-      <c r="F6" s="1">
-        <f t="shared" si="0"/>
-        <v>0.66669619073718833</v>
-      </c>
-      <c r="G6" s="1">
-        <f t="shared" si="0"/>
-        <v>0.77553327766715907</v>
+        <v>0.67108101336799153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>